<commit_message>
Adding E-Mail anonymizer based on manually created Excel file, first try to train Model based on BERT
</commit_message>
<xml_diff>
--- a/data/DAiA Manual Labeling.xlsx
+++ b/data/DAiA Manual Labeling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3255aa3fa7d48a59/Desktop/Veranstaltungen/Data Analytics in Applications/daia-eon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{114ED53A-7DD9-4EBE-ACAF-8801673E5573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C55EED3E-D390-8945-8EF2-AA09107EAC97}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{114ED53A-7DD9-4EBE-ACAF-8801673E5573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9140542-6BB2-0D4F-93AF-5C29EA8E13F2}"/>
   <bookViews>
-    <workbookView xWindow="19580" yWindow="22520" windowWidth="14480" windowHeight="16620" xr2:uid="{D5A5125A-2A0E-AE4B-B7B2-07D8AB5715C0}"/>
+    <workbookView xWindow="14780" yWindow="900" windowWidth="14440" windowHeight="16640" xr2:uid="{D5A5125A-2A0E-AE4B-B7B2-07D8AB5715C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3472,11 +3472,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF80886-0555-0A47-A890-09D645E2269F}">
   <dimension ref="A1:BE161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="W127" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB146" sqref="AB146"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>